<commit_message>
imputation relationship between RGRcambiummax and SRsapwood
</commit_message>
<xml_diff>
--- a/data-raw/SpParamsMED.xlsx
+++ b/data-raw/SpParamsMED.xlsx
@@ -3568,7 +3568,7 @@
       <c r="DA2"/>
       <c r="DB2"/>
       <c r="DC2" t="n">
-        <v>0.009</v>
+        <v>0.00436884567569464</v>
       </c>
       <c r="DD2"/>
       <c r="DE2"/>
@@ -3836,7 +3836,7 @@
       <c r="DA3"/>
       <c r="DB3"/>
       <c r="DC3" t="n">
-        <v>0.00541140413646241</v>
+        <v>0.0112038218493728</v>
       </c>
       <c r="DD3"/>
       <c r="DE3"/>
@@ -4059,7 +4059,9 @@
       <c r="CZ4"/>
       <c r="DA4"/>
       <c r="DB4"/>
-      <c r="DC4"/>
+      <c r="DC4" t="n">
+        <v>0.00580578341790764</v>
+      </c>
       <c r="DD4"/>
       <c r="DE4"/>
       <c r="DF4"/>
@@ -4326,7 +4328,7 @@
       <c r="DA5"/>
       <c r="DB5"/>
       <c r="DC5" t="n">
-        <v>0.0018</v>
+        <v>0.00332747264670449</v>
       </c>
       <c r="DD5"/>
       <c r="DE5"/>
@@ -4596,7 +4598,7 @@
       <c r="DA6"/>
       <c r="DB6"/>
       <c r="DC6" t="n">
-        <v>0.00104629510698032</v>
+        <v>0.00223051546972426</v>
       </c>
       <c r="DD6"/>
       <c r="DE6"/>
@@ -4866,7 +4868,7 @@
       <c r="DA7"/>
       <c r="DB7"/>
       <c r="DC7" t="n">
-        <v>0.00342109137573859</v>
+        <v>0.00711235790822628</v>
       </c>
       <c r="DD7"/>
       <c r="DE7"/>
@@ -5132,7 +5134,7 @@
       <c r="DA8"/>
       <c r="DB8"/>
       <c r="DC8" t="n">
-        <v>0.00170652309252545</v>
+        <v>0.0035877388413974</v>
       </c>
       <c r="DD8"/>
       <c r="DE8"/>
@@ -5402,7 +5404,7 @@
       <c r="DA9"/>
       <c r="DB9"/>
       <c r="DC9" t="n">
-        <v>0.00197513529743135</v>
+        <v>0.00413992198176206</v>
       </c>
       <c r="DD9"/>
       <c r="DE9"/>
@@ -5668,7 +5670,7 @@
       <c r="DA10"/>
       <c r="DB10"/>
       <c r="DC10" t="n">
-        <v>0.00201619115607833</v>
+        <v>0.00422432005654799</v>
       </c>
       <c r="DD10"/>
       <c r="DE10"/>
@@ -6276,7 +6278,7 @@
       <c r="DA13"/>
       <c r="DB13"/>
       <c r="DC13" t="n">
-        <v>0.0020664773002519</v>
+        <v>0.0043276927272586</v>
       </c>
       <c r="DD13"/>
       <c r="DE13"/>
@@ -7375,7 +7377,9 @@
       <c r="CZ19"/>
       <c r="DA19"/>
       <c r="DB19"/>
-      <c r="DC19"/>
+      <c r="DC19" t="n">
+        <v>0.00538354422116695</v>
+      </c>
       <c r="DD19"/>
       <c r="DE19"/>
       <c r="DF19"/>
@@ -7591,7 +7595,9 @@
       <c r="CZ20"/>
       <c r="DA20"/>
       <c r="DB20"/>
-      <c r="DC20"/>
+      <c r="DC20" t="n">
+        <v>0.00179411628687287</v>
+      </c>
       <c r="DD20"/>
       <c r="DE20"/>
       <c r="DF20"/>
@@ -7810,7 +7816,7 @@
       <c r="DA21"/>
       <c r="DB21"/>
       <c r="DC21" t="n">
-        <v>0.00075</v>
+        <v>0.00211563236280096</v>
       </c>
       <c r="DD21"/>
       <c r="DE21"/>
@@ -9302,7 +9308,7 @@
       <c r="DA28"/>
       <c r="DB28"/>
       <c r="DC28" t="n">
-        <v>0.003</v>
+        <v>0.00214517820971025</v>
       </c>
       <c r="DD28"/>
       <c r="DE28"/>
@@ -9718,7 +9724,7 @@
       <c r="DA30"/>
       <c r="DB30"/>
       <c r="DC30" t="n">
-        <v>0.000805386302436502</v>
+        <v>0.00173528190324836</v>
       </c>
       <c r="DD30"/>
       <c r="DE30"/>
@@ -10560,7 +10566,7 @@
       <c r="DA34"/>
       <c r="DB34"/>
       <c r="DC34" t="n">
-        <v>0.0033</v>
+        <v>0.00406142526617734</v>
       </c>
       <c r="DD34"/>
       <c r="DE34"/>
@@ -10786,7 +10792,7 @@
       <c r="DA35"/>
       <c r="DB35"/>
       <c r="DC35" t="n">
-        <v>0.00410743851571631</v>
+        <v>0.00852327413694334</v>
       </c>
       <c r="DD35"/>
       <c r="DE35"/>
@@ -10998,7 +11004,7 @@
       <c r="DA36"/>
       <c r="DB36"/>
       <c r="DC36" t="n">
-        <v>0.00263627952336136</v>
+        <v>0.00549902885866622</v>
       </c>
       <c r="DD36"/>
       <c r="DE36"/>
@@ -11206,7 +11212,7 @@
       <c r="DA37"/>
       <c r="DB37"/>
       <c r="DC37" t="n">
-        <v>0.00114683417221073</v>
+        <v>0.00243719251475169</v>
       </c>
       <c r="DD37"/>
       <c r="DE37"/>
@@ -11399,7 +11405,9 @@
       <c r="CZ38"/>
       <c r="DA38"/>
       <c r="DB38"/>
-      <c r="DC38"/>
+      <c r="DC38" t="n">
+        <v>0.00809450440777297</v>
+      </c>
       <c r="DD38"/>
       <c r="DE38"/>
       <c r="DF38"/>
@@ -15936,7 +15944,7 @@
       <c r="DA60"/>
       <c r="DB60"/>
       <c r="DC60" t="n">
-        <v>0.00074532289803413</v>
+        <v>0.00161181022676399</v>
       </c>
       <c r="DD60"/>
       <c r="DE60"/>
@@ -16346,7 +16354,7 @@
       <c r="DA62"/>
       <c r="DB62"/>
       <c r="DC62" t="n">
-        <v>0.0045</v>
+        <v>0.00160939061023085</v>
       </c>
       <c r="DD62"/>
       <c r="DE62"/>
@@ -16562,7 +16570,7 @@
       <c r="DA63"/>
       <c r="DB63"/>
       <c r="DC63" t="n">
-        <v>0.00190596751156624</v>
+        <v>0.0039977345289453</v>
       </c>
       <c r="DD63"/>
       <c r="DE63"/>
@@ -20893,7 +20901,9 @@
       <c r="CZ85"/>
       <c r="DA85"/>
       <c r="DB85"/>
-      <c r="DC85"/>
+      <c r="DC85" t="n">
+        <v>0.00209934449788569</v>
+      </c>
       <c r="DD85"/>
       <c r="DE85"/>
       <c r="DF85"/>
@@ -22177,7 +22187,9 @@
       <c r="CZ91"/>
       <c r="DA91"/>
       <c r="DB91"/>
-      <c r="DC91"/>
+      <c r="DC91" t="n">
+        <v>0.0032480944379835</v>
+      </c>
       <c r="DD91"/>
       <c r="DE91"/>
       <c r="DF91"/>
@@ -23238,7 +23250,7 @@
       <c r="DA96"/>
       <c r="DB96"/>
       <c r="DC96" t="n">
-        <v>0.00446026223217329</v>
+        <v>0.00647655185474176</v>
       </c>
       <c r="DD96"/>
       <c r="DE96"/>
@@ -23437,7 +23449,9 @@
       <c r="CZ97"/>
       <c r="DA97"/>
       <c r="DB97"/>
-      <c r="DC97"/>
+      <c r="DC97" t="n">
+        <v>0.00192088952434155</v>
+      </c>
       <c r="DD97"/>
       <c r="DE97"/>
       <c r="DF97"/>
@@ -23926,7 +23940,7 @@
       <c r="DA99"/>
       <c r="DB99"/>
       <c r="DC99" t="n">
-        <v>0.00287045527228856</v>
+        <v>0.00393961812729256</v>
       </c>
       <c r="DD99"/>
       <c r="DE99"/>
@@ -24146,7 +24160,7 @@
       <c r="DA100"/>
       <c r="DB100"/>
       <c r="DC100" t="n">
-        <v>0.00104102511675227</v>
+        <v>0.00221968200906733</v>
       </c>
       <c r="DD100"/>
       <c r="DE100"/>
@@ -24343,7 +24357,9 @@
       <c r="CZ101"/>
       <c r="DA101"/>
       <c r="DB101"/>
-      <c r="DC101"/>
+      <c r="DC101" t="n">
+        <v>0.00207460512683456</v>
+      </c>
       <c r="DD101"/>
       <c r="DE101"/>
       <c r="DF101"/>
@@ -24582,7 +24598,7 @@
       <c r="DA102"/>
       <c r="DB102"/>
       <c r="DC102" t="n">
-        <v>0.00286683104357139</v>
+        <v>0.00393383476597852</v>
       </c>
       <c r="DD102"/>
       <c r="DE102"/>
@@ -25687,7 +25703,9 @@
       <c r="CZ108"/>
       <c r="DA108"/>
       <c r="DB108"/>
-      <c r="DC108"/>
+      <c r="DC108" t="n">
+        <v>0.00154888215417536</v>
+      </c>
       <c r="DD108"/>
       <c r="DE108"/>
       <c r="DF108"/>
@@ -26722,7 +26740,7 @@
       <c r="DA113"/>
       <c r="DB113"/>
       <c r="DC113" t="n">
-        <v>0.000922875020622103</v>
+        <v>0.00197680216249298</v>
       </c>
       <c r="DD113"/>
       <c r="DE113"/>
@@ -27130,7 +27148,7 @@
       <c r="DA115"/>
       <c r="DB115"/>
       <c r="DC115" t="n">
-        <v>0.00269474892541116</v>
+        <v>0.00365923480480888</v>
       </c>
       <c r="DD115"/>
       <c r="DE115"/>
@@ -27357,7 +27375,9 @@
       <c r="CZ116"/>
       <c r="DA116"/>
       <c r="DB116"/>
-      <c r="DC116"/>
+      <c r="DC116" t="n">
+        <v>0.0097784699464709</v>
+      </c>
       <c r="DD116"/>
       <c r="DE116"/>
       <c r="DF116"/>
@@ -27596,7 +27616,7 @@
       <c r="DA117"/>
       <c r="DB117"/>
       <c r="DC117" t="n">
-        <v>0.000679791900724173</v>
+        <v>0.00147709887997869</v>
       </c>
       <c r="DD117"/>
       <c r="DE117"/>
@@ -27850,7 +27870,7 @@
       <c r="DA118"/>
       <c r="DB118"/>
       <c r="DC118" t="n">
-        <v>0.000775490619980894</v>
+        <v>0.00167382567929358</v>
       </c>
       <c r="DD118"/>
       <c r="DE118"/>
@@ -28104,7 +28124,7 @@
       <c r="DA119"/>
       <c r="DB119"/>
       <c r="DC119" t="n">
-        <v>0.000670305107362669</v>
+        <v>0.00145759698373321</v>
       </c>
       <c r="DD119"/>
       <c r="DE119"/>
@@ -28344,7 +28364,7 @@
       <c r="DA120"/>
       <c r="DB120"/>
       <c r="DC120" t="n">
-        <v>0.000773867908124838</v>
+        <v>0.00167048988846867</v>
       </c>
       <c r="DD120"/>
       <c r="DE120"/>
@@ -28740,7 +28760,7 @@
       <c r="DA122"/>
       <c r="DB122"/>
       <c r="DC122" t="n">
-        <v>0.00250034335645265</v>
+        <v>0.00521958638300106</v>
       </c>
       <c r="DD122"/>
       <c r="DE122"/>
@@ -29143,7 +29163,9 @@
       <c r="CZ124"/>
       <c r="DA124"/>
       <c r="DB124"/>
-      <c r="DC124"/>
+      <c r="DC124" t="n">
+        <v>0.00391492046474905</v>
+      </c>
       <c r="DD124"/>
       <c r="DE124"/>
       <c r="DF124"/>
@@ -30152,7 +30174,7 @@
       <c r="DA129"/>
       <c r="DB129"/>
       <c r="DC129" t="n">
-        <v>0.000983367873404511</v>
+        <v>0.00210115665126504</v>
       </c>
       <c r="DD129"/>
       <c r="DE129"/>
@@ -30745,7 +30767,9 @@
       <c r="CZ132"/>
       <c r="DA132"/>
       <c r="DB132"/>
-      <c r="DC132"/>
+      <c r="DC132" t="n">
+        <v>0.000906464250099299</v>
+      </c>
       <c r="DD132"/>
       <c r="DE132"/>
       <c r="DF132"/>
@@ -30937,7 +30961,9 @@
       <c r="CZ133"/>
       <c r="DA133"/>
       <c r="DB133"/>
-      <c r="DC133"/>
+      <c r="DC133" t="n">
+        <v>0.00228755864896635</v>
+      </c>
       <c r="DD133"/>
       <c r="DE133"/>
       <c r="DF133"/>
@@ -31786,7 +31812,7 @@
       <c r="DA137"/>
       <c r="DB137"/>
       <c r="DC137" t="n">
-        <v>0.000561195094839645</v>
+        <v>0.00123330073710027</v>
       </c>
       <c r="DD137"/>
       <c r="DE137"/>
@@ -32735,7 +32761,9 @@
       <c r="CZ142"/>
       <c r="DA142"/>
       <c r="DB142"/>
-      <c r="DC142"/>
+      <c r="DC142" t="n">
+        <v>0.00482291903325982</v>
+      </c>
       <c r="DD142"/>
       <c r="DE142"/>
       <c r="DF142"/>
@@ -33176,7 +33204,7 @@
       <c r="DA144"/>
       <c r="DB144"/>
       <c r="DC144" t="n">
-        <v>0.000845588709140148</v>
+        <v>0.00181792554630848</v>
       </c>
       <c r="DD144"/>
       <c r="DE144"/>
@@ -33559,7 +33587,9 @@
       <c r="CZ146"/>
       <c r="DA146"/>
       <c r="DB146"/>
-      <c r="DC146"/>
+      <c r="DC146" t="n">
+        <v>0.000388710737531233</v>
+      </c>
       <c r="DD146"/>
       <c r="DE146"/>
       <c r="DF146"/>
@@ -33737,7 +33767,9 @@
       <c r="CZ147"/>
       <c r="DA147"/>
       <c r="DB147"/>
-      <c r="DC147"/>
+      <c r="DC147" t="n">
+        <v>0.00510170460598088</v>
+      </c>
       <c r="DD147"/>
       <c r="DE147"/>
       <c r="DF147"/>
@@ -33984,7 +34016,7 @@
       <c r="DA148"/>
       <c r="DB148"/>
       <c r="DC148" t="n">
-        <v>0.00298912793143386</v>
+        <v>0.00622437543072686</v>
       </c>
       <c r="DD148"/>
       <c r="DE148"/>
@@ -34233,7 +34265,9 @@
       </c>
       <c r="DA149"/>
       <c r="DB149"/>
-      <c r="DC149"/>
+      <c r="DC149" t="n">
+        <v>0.00277222661670983</v>
+      </c>
       <c r="DD149"/>
       <c r="DE149"/>
       <c r="DF149"/>
@@ -34514,7 +34548,7 @@
       <c r="DA150"/>
       <c r="DB150"/>
       <c r="DC150" t="n">
-        <v>0.00247516722331096</v>
+        <v>0.0048701782840047</v>
       </c>
       <c r="DD150"/>
       <c r="DE150"/>
@@ -34808,7 +34842,7 @@
       <c r="DA151"/>
       <c r="DB151"/>
       <c r="DC151" t="n">
-        <v>0.00182427252412565</v>
+        <v>0.00377037027023632</v>
       </c>
       <c r="DD151"/>
       <c r="DE151"/>
@@ -35068,7 +35102,7 @@
       <c r="DA152"/>
       <c r="DB152"/>
       <c r="DC152" t="n">
-        <v>0.007</v>
+        <v>0.00683210209777577</v>
       </c>
       <c r="DD152"/>
       <c r="DE152"/>
@@ -35350,7 +35384,7 @@
       <c r="DA153"/>
       <c r="DB153"/>
       <c r="DC153" t="n">
-        <v>0.00249418909410628</v>
+        <v>0.00490842611647506</v>
       </c>
       <c r="DD153"/>
       <c r="DE153"/>
@@ -35610,7 +35644,7 @@
       <c r="DA154"/>
       <c r="DB154"/>
       <c r="DC154" t="n">
-        <v>0.00864654403075331</v>
+        <v>0.00970727844740331</v>
       </c>
       <c r="DD154"/>
       <c r="DE154"/>
@@ -35904,7 +35938,7 @@
       <c r="DA155"/>
       <c r="DB155"/>
       <c r="DC155" t="n">
-        <v>0.00318642248360167</v>
+        <v>0.00387104310336164</v>
       </c>
       <c r="DD155"/>
       <c r="DE155"/>
@@ -36186,7 +36220,7 @@
       <c r="DA156"/>
       <c r="DB156"/>
       <c r="DC156" t="n">
-        <v>0.0045</v>
+        <v>0.00301220197523165</v>
       </c>
       <c r="DD156"/>
       <c r="DE156"/>
@@ -36856,7 +36890,7 @@
       <c r="DA159"/>
       <c r="DB159"/>
       <c r="DC159" t="n">
-        <v>0.000864733893415942</v>
+        <v>0.00185728208999186</v>
       </c>
       <c r="DD159"/>
       <c r="DE159"/>
@@ -37068,7 +37102,7 @@
       <c r="DA160"/>
       <c r="DB160"/>
       <c r="DC160" t="n">
-        <v>0.00490976185432422</v>
+        <v>0.00719384067073301</v>
       </c>
       <c r="DD160"/>
       <c r="DE160"/>
@@ -37466,7 +37500,7 @@
       <c r="DA162"/>
       <c r="DB162"/>
       <c r="DC162" t="n">
-        <v>0.007</v>
+        <v>0.00587442682512847</v>
       </c>
       <c r="DD162"/>
       <c r="DE162"/>
@@ -37722,7 +37756,7 @@
       <c r="DA163"/>
       <c r="DB163"/>
       <c r="DC163" t="n">
-        <v>0.00256836245980357</v>
+        <v>0.00345755366025266</v>
       </c>
       <c r="DD163"/>
       <c r="DE163"/>
@@ -37966,7 +38000,7 @@
       <c r="DA164"/>
       <c r="DB164"/>
       <c r="DC164" t="n">
-        <v>0.00478099525379898</v>
+        <v>0.00990789727787083</v>
       </c>
       <c r="DD164"/>
       <c r="DE164"/>
@@ -38168,7 +38202,7 @@
       <c r="DA165"/>
       <c r="DB165"/>
       <c r="DC165" t="n">
-        <v>0.00149855827982982</v>
+        <v>0.00316022787479836</v>
       </c>
       <c r="DD165"/>
       <c r="DE165"/>
@@ -38450,7 +38484,7 @@
       <c r="DA166"/>
       <c r="DB166"/>
       <c r="DC166" t="n">
-        <v>0.00188401951890941</v>
+        <v>0.00478993927234319</v>
       </c>
       <c r="DD166"/>
       <c r="DE166"/>
@@ -39014,7 +39048,7 @@
       <c r="DA168"/>
       <c r="DB168"/>
       <c r="DC168" t="n">
-        <v>0.00120315572719097</v>
+        <v>0.00303513046077045</v>
       </c>
       <c r="DD168"/>
       <c r="DE168"/>
@@ -39592,7 +39626,7 @@
       <c r="DA170"/>
       <c r="DB170"/>
       <c r="DC170" t="n">
-        <v>0.00065</v>
+        <v>0.00252987678197495</v>
       </c>
       <c r="DD170"/>
       <c r="DE170"/>
@@ -40144,7 +40178,7 @@
       <c r="DA172"/>
       <c r="DB172"/>
       <c r="DC172" t="n">
-        <v>0.00124700238778517</v>
+        <v>0.00314813765443329</v>
       </c>
       <c r="DD172"/>
       <c r="DE172"/>
@@ -40450,7 +40484,7 @@
       <c r="DA173"/>
       <c r="DB173"/>
       <c r="DC173" t="n">
-        <v>0.00116489773657126</v>
+        <v>0.0029365270985868</v>
       </c>
       <c r="DD173"/>
       <c r="DE173"/>
@@ -40734,7 +40768,7 @@
       <c r="DA174"/>
       <c r="DB174"/>
       <c r="DC174" t="n">
-        <v>0.00138903037021725</v>
+        <v>0.0035141902454114</v>
       </c>
       <c r="DD174"/>
       <c r="DE174"/>
@@ -41032,7 +41066,7 @@
       <c r="DA175"/>
       <c r="DB175"/>
       <c r="DC175" t="n">
-        <v>0.00180705659611069</v>
+        <v>0.00459158063331096</v>
       </c>
       <c r="DD175"/>
       <c r="DE175"/>
@@ -41316,7 +41350,7 @@
       <c r="DA176"/>
       <c r="DB176"/>
       <c r="DC176" t="n">
-        <v>0.00125128849766263</v>
+        <v>0.00315918436226506</v>
       </c>
       <c r="DD176"/>
       <c r="DE176"/>
@@ -41622,7 +41656,7 @@
       <c r="DA177"/>
       <c r="DB177"/>
       <c r="DC177" t="n">
-        <v>0.00075</v>
+        <v>0.00258763899591654</v>
       </c>
       <c r="DD177"/>
       <c r="DE177"/>
@@ -42050,7 +42084,7 @@
       <c r="DA179"/>
       <c r="DB179"/>
       <c r="DC179" t="n">
-        <v>0.00109286247939468</v>
+        <v>0.00232624350243706</v>
       </c>
       <c r="DD179"/>
       <c r="DE179"/>
@@ -42898,7 +42932,7 @@
       <c r="DA183"/>
       <c r="DB183"/>
       <c r="DC183" t="n">
-        <v>0.00286424147522188</v>
+        <v>0.00596764772319659</v>
       </c>
       <c r="DD183"/>
       <c r="DE183"/>
@@ -43976,7 +44010,7 @@
       <c r="DA188"/>
       <c r="DB188"/>
       <c r="DC188" t="n">
-        <v>0.00161739483068106</v>
+        <v>0.00340451885875469</v>
       </c>
       <c r="DD188"/>
       <c r="DE188"/>
@@ -44606,7 +44640,7 @@
       <c r="DA191"/>
       <c r="DB191"/>
       <c r="DC191" t="n">
-        <v>0.00275307686981761</v>
+        <v>0.00573912787268931</v>
       </c>
       <c r="DD191"/>
       <c r="DE191"/>
@@ -45882,7 +45916,7 @@
       <c r="DA198"/>
       <c r="DB198"/>
       <c r="DC198" t="n">
-        <v>0.004</v>
+        <v>0.00241091331463683</v>
       </c>
       <c r="DD198"/>
       <c r="DE198"/>
@@ -46457,7 +46491,9 @@
       <c r="CZ201"/>
       <c r="DA201"/>
       <c r="DB201"/>
-      <c r="DC201"/>
+      <c r="DC201" t="n">
+        <v>0.00366147808461013</v>
+      </c>
       <c r="DD201"/>
       <c r="DE201"/>
       <c r="DF201"/>
@@ -46684,7 +46720,7 @@
       <c r="DA202"/>
       <c r="DB202"/>
       <c r="DC202" t="n">
-        <v>0.000625044411359914</v>
+        <v>0.00136455507127563</v>
       </c>
       <c r="DD202"/>
       <c r="DE202"/>
@@ -47455,7 +47491,9 @@
       <c r="CZ206"/>
       <c r="DA206"/>
       <c r="DB206"/>
-      <c r="DC206"/>
+      <c r="DC206" t="n">
+        <v>0.00151751058415808</v>
+      </c>
       <c r="DD206"/>
       <c r="DE206"/>
       <c r="DF206"/>
@@ -48064,7 +48102,7 @@
       <c r="DA209"/>
       <c r="DB209"/>
       <c r="DC209" t="n">
-        <v>0.007</v>
+        <v>0.00406479631224623</v>
       </c>
       <c r="DD209"/>
       <c r="DE209"/>
@@ -48478,7 +48516,7 @@
       <c r="DA211"/>
       <c r="DB211"/>
       <c r="DC211" t="n">
-        <v>0.00118395501236878</v>
+        <v>0.00251350141552791</v>
       </c>
       <c r="DD211"/>
       <c r="DE211"/>

</xml_diff>